<commit_message>
create appendix for definitions, refine a bit description of annotations
</commit_message>
<xml_diff>
--- a/assets/definitions.xlsx
+++ b/assets/definitions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u0118974\OneDrive - KU Leuven\repos\montesmariana\phdThesis\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7089A722-003B-4BAE-8A34-7B230E51297F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A8EECE0-1CD0-472A-9866-510D8D682AA9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="779" uniqueCount="681">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="786" uniqueCount="681">
   <si>
     <t>code</t>
   </si>
@@ -2414,8 +2414,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L139"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A129" workbookViewId="0">
+      <selection activeCell="D140" sqref="D140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2423,7 +2423,7 @@
     <col min="1" max="1" width="16.08984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38.54296875" customWidth="1"/>
     <col min="3" max="3" width="35.36328125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="3.36328125" customWidth="1"/>
+    <col min="4" max="4" width="13.36328125" customWidth="1"/>
     <col min="5" max="5" width="6.1796875" customWidth="1"/>
     <col min="6" max="6" width="12.81640625" customWidth="1"/>
     <col min="7" max="8" width="7.1796875" customWidth="1"/>
@@ -2632,6 +2632,9 @@
       <c r="A6" t="s">
         <v>676</v>
       </c>
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
       <c r="E6">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -7588,6 +7591,9 @@
       <c r="A134" t="s">
         <v>497</v>
       </c>
+      <c r="D134" t="s">
+        <v>396</v>
+      </c>
       <c r="J134" t="s">
         <v>507</v>
       </c>
@@ -7602,6 +7608,9 @@
       <c r="A135" t="s">
         <v>498</v>
       </c>
+      <c r="D135" t="s">
+        <v>358</v>
+      </c>
       <c r="J135" t="s">
         <v>500</v>
       </c>
@@ -7616,6 +7625,9 @@
       <c r="A136" t="s">
         <v>504</v>
       </c>
+      <c r="D136" t="s">
+        <v>358</v>
+      </c>
       <c r="J136" t="s">
         <v>499</v>
       </c>
@@ -7630,6 +7642,9 @@
       <c r="A137" t="s">
         <v>309</v>
       </c>
+      <c r="D137" t="s">
+        <v>305</v>
+      </c>
       <c r="J137" t="s">
         <v>501</v>
       </c>
@@ -7644,6 +7659,9 @@
       <c r="A138" t="s">
         <v>502</v>
       </c>
+      <c r="D138" t="s">
+        <v>315</v>
+      </c>
       <c r="J138" t="s">
         <v>503</v>
       </c>
@@ -7657,6 +7675,9 @@
     <row r="139" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>506</v>
+      </c>
+      <c r="D139" t="s">
+        <v>273</v>
       </c>
       <c r="J139" t="s">
         <v>505</v>

</xml_diff>

<commit_message>
Design comments and translate examples
</commit_message>
<xml_diff>
--- a/assets/definitions.xlsx
+++ b/assets/definitions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u0118974\OneDrive - KU Leuven\repos\montesmariana\phdThesis\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A8EECE0-1CD0-472A-9866-510D8D682AA9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A85C7E5-88CC-4EB7-BA2F-B603303BDDE4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="786" uniqueCount="681">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="783" uniqueCount="680">
   <si>
     <t>code</t>
   </si>
@@ -1352,9 +1352,6 @@
     <t>history repeats itself</t>
   </si>
   <si>
-    <t>(with _aan_ 'of') bring back to the mind, to the memory</t>
-  </si>
-  <si>
     <t>remind someone of something</t>
   </si>
   <si>
@@ -1502,9 +1499,6 @@
     <t>he was made to trip in the penalty kick, make someone trip</t>
   </si>
   <si>
-    <t>(intrans., with _blijven_ 'keep') of thoughts, gazes and such: falter, come back (to something)</t>
-  </si>
-  <si>
     <t>I kept going back to the memory of my brother</t>
   </si>
   <si>
@@ -1544,15 +1538,9 @@
     <t>helpen_4</t>
   </si>
   <si>
-    <t>(with _aan_) provide</t>
-  </si>
-  <si>
     <t>(trans.) with inanimate entities, be helpful, useful</t>
   </si>
   <si>
-    <t>(trans.) in the construction "herinnered worden als", keep in the collective memory</t>
-  </si>
-  <si>
     <t>herhalen_4</t>
   </si>
   <si>
@@ -1568,9 +1556,6 @@
     <t>herstellen_6</t>
   </si>
   <si>
-    <t>(with _naar_ 'to') desire, aim for</t>
-  </si>
-  <si>
     <t>a hopeful mood, that brings me hope (makes me hopeful)</t>
   </si>
   <si>
@@ -1604,9 +1589,6 @@
     <t>a dangerous situation</t>
   </si>
   <si>
-    <t>(really) dangerous, trick, critical, dire</t>
-  </si>
-  <si>
     <t>an angulous drawing, an angulous face</t>
   </si>
   <si>
@@ -1652,27 +1634,15 @@
     <t>a healthy diet</t>
   </si>
   <si>
-    <t>(literal) that brings health and physical wellbeing</t>
-  </si>
-  <si>
     <t>a beneficial decision</t>
   </si>
   <si>
-    <t>(figurative) necessary, having a beneficial effect</t>
-  </si>
-  <si>
     <t>colored cheeks</t>
   </si>
   <si>
-    <t>with color, in a literal sense (in particular, not black, white or gray)</t>
-  </si>
-  <si>
     <t>the fellow colored man, to be of colored origin</t>
   </si>
   <si>
-    <t>(of people and related) not white</t>
-  </si>
-  <si>
     <t>a colored representation of things</t>
   </si>
   <si>
@@ -1913,9 +1883,6 @@
     <t>Spot</t>
   </si>
   <si>
-    <t>(section of a magazine?)</t>
-  </si>
-  <si>
     <t>twelve tons of steel, iron and steel, man of steel</t>
   </si>
   <si>
@@ -1994,9 +1961,6 @@
     <t>lift up dust</t>
   </si>
   <si>
-    <t>2.3 idiomatic uses of "dust"</t>
-  </si>
-  <si>
     <t>a ferocious horde</t>
   </si>
   <si>
@@ -2066,9 +2030,6 @@
     <t>gemeen_6</t>
   </si>
   <si>
-    <t>cool, awesome, badass?</t>
-  </si>
-  <si>
     <t>pilot_n</t>
   </si>
   <si>
@@ -2081,13 +2042,49 @@
     <t>I find this funny</t>
   </si>
   <si>
-    <t>be perceived as funny (and witty?)</t>
-  </si>
-  <si>
-    <t>popular, interesting/new, recent</t>
-  </si>
-  <si>
     <t>a bunch of people, a lot of money</t>
+  </si>
+  <si>
+    <t>(intrans., with 'to keep') of thoughts, gazes and such: falter, come back (to something)</t>
+  </si>
+  <si>
+    <t>(with 'towards') desire, aim for</t>
+  </si>
+  <si>
+    <t>(with 'to/for') to provide</t>
+  </si>
+  <si>
+    <t>(with 'of') bring back to the mind, to the memory</t>
+  </si>
+  <si>
+    <t>being perceived as witty</t>
+  </si>
+  <si>
+    <t>(actually) dangerous, trick, critical, dire</t>
+  </si>
+  <si>
+    <t>(lit.) that brings health and physical wellbeing</t>
+  </si>
+  <si>
+    <t>(fig.) necessary, having a beneficial effect</t>
+  </si>
+  <si>
+    <t>with colour, in a literal sense (in particular, not black, white or gray)</t>
+  </si>
+  <si>
+    <t>(of people a.o.) not white</t>
+  </si>
+  <si>
+    <t>popular, interesting or new, recent</t>
+  </si>
+  <si>
+    <t>cool, awesome, badass</t>
+  </si>
+  <si>
+    <t>(headline usage)</t>
+  </si>
+  <si>
+    <t>2.3 idiomatic uses of 'dust'</t>
   </si>
 </sst>
 </file>
@@ -2412,10 +2409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L139"/>
+  <dimension ref="A1:L138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A129" workbookViewId="0">
-      <selection activeCell="D140" sqref="D140"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2427,7 +2424,7 @@
     <col min="5" max="5" width="6.1796875" customWidth="1"/>
     <col min="6" max="6" width="12.81640625" customWidth="1"/>
     <col min="7" max="8" width="7.1796875" customWidth="1"/>
-    <col min="10" max="10" width="49.90625" customWidth="1"/>
+    <col min="10" max="10" width="49.90625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.35">
@@ -2447,10 +2444,10 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>675</v>
+        <v>662</v>
       </c>
       <c r="G1" t="s">
-        <v>674</v>
+        <v>661</v>
       </c>
       <c r="H1" t="s">
         <v>5</v>
@@ -2458,14 +2455,14 @@
       <c r="I1" t="s">
         <v>409</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>410</v>
       </c>
       <c r="K1" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="L1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
@@ -2496,10 +2493,10 @@
         <v>24</v>
       </c>
       <c r="I2" t="s">
-        <v>508</v>
-      </c>
-      <c r="J2" t="s">
-        <v>509</v>
+        <v>503</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>504</v>
       </c>
       <c r="K2" t="b">
         <v>1</v>
@@ -2536,10 +2533,10 @@
         <v>12</v>
       </c>
       <c r="I3" t="s">
-        <v>510</v>
-      </c>
-      <c r="J3" t="s">
-        <v>511</v>
+        <v>505</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>506</v>
       </c>
       <c r="K3" t="b">
         <v>1</v>
@@ -2576,10 +2573,10 @@
         <v>6</v>
       </c>
       <c r="I4" t="s">
-        <v>512</v>
-      </c>
-      <c r="J4" t="s">
-        <v>513</v>
+        <v>507</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>508</v>
       </c>
       <c r="K4" t="b">
         <v>1</v>
@@ -2616,10 +2613,10 @@
         <v>32</v>
       </c>
       <c r="I5" t="s">
-        <v>514</v>
-      </c>
-      <c r="J5" t="s">
-        <v>515</v>
+        <v>509</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>510</v>
       </c>
       <c r="K5" t="b">
         <v>1</v>
@@ -2630,7 +2627,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>676</v>
+        <v>663</v>
       </c>
       <c r="D6" t="s">
         <v>16</v>
@@ -2650,10 +2647,10 @@
         <v>0</v>
       </c>
       <c r="I6" t="s">
-        <v>677</v>
-      </c>
-      <c r="J6" t="s">
-        <v>678</v>
+        <v>664</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>670</v>
       </c>
       <c r="K6" t="b">
         <v>0</v>
@@ -2690,10 +2687,10 @@
         <v>23</v>
       </c>
       <c r="I7" t="s">
-        <v>516</v>
-      </c>
-      <c r="J7" t="s">
-        <v>517</v>
+        <v>511</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>512</v>
       </c>
       <c r="K7" t="b">
         <v>1</v>
@@ -2730,10 +2727,10 @@
         <v>16</v>
       </c>
       <c r="I8" t="s">
-        <v>518</v>
-      </c>
-      <c r="J8" t="s">
-        <v>519</v>
+        <v>513</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>671</v>
       </c>
       <c r="K8" t="b">
         <v>1</v>
@@ -2770,10 +2767,10 @@
         <v>19</v>
       </c>
       <c r="I9" t="s">
-        <v>520</v>
-      </c>
-      <c r="J9" t="s">
-        <v>521</v>
+        <v>514</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>515</v>
       </c>
       <c r="K9" t="b">
         <v>1</v>
@@ -2810,10 +2807,10 @@
         <v>11</v>
       </c>
       <c r="I10" t="s">
-        <v>522</v>
-      </c>
-      <c r="J10" t="s">
-        <v>523</v>
+        <v>516</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>517</v>
       </c>
       <c r="K10" t="b">
         <v>1</v>
@@ -2850,10 +2847,10 @@
         <v>5</v>
       </c>
       <c r="I11" t="s">
-        <v>524</v>
-      </c>
-      <c r="J11" t="s">
-        <v>525</v>
+        <v>518</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>519</v>
       </c>
       <c r="K11" t="b">
         <v>1</v>
@@ -2890,10 +2887,10 @@
         <v>12</v>
       </c>
       <c r="I12" t="s">
-        <v>526</v>
-      </c>
-      <c r="J12" t="s">
-        <v>527</v>
+        <v>520</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>521</v>
       </c>
       <c r="K12" t="b">
         <v>1</v>
@@ -2930,10 +2927,10 @@
         <v>12</v>
       </c>
       <c r="I13" t="s">
-        <v>528</v>
-      </c>
-      <c r="J13" t="s">
-        <v>529</v>
+        <v>522</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>523</v>
       </c>
       <c r="K13" t="b">
         <v>1</v>
@@ -2970,10 +2967,10 @@
         <v>8</v>
       </c>
       <c r="I14" t="s">
-        <v>530</v>
-      </c>
-      <c r="J14" t="s">
-        <v>531</v>
+        <v>524</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>525</v>
       </c>
       <c r="K14" t="b">
         <v>1</v>
@@ -3010,10 +3007,10 @@
         <v>2</v>
       </c>
       <c r="I15" t="s">
-        <v>532</v>
-      </c>
-      <c r="J15" t="s">
-        <v>533</v>
+        <v>526</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>527</v>
       </c>
       <c r="K15" t="b">
         <v>1</v>
@@ -3050,10 +3047,10 @@
         <v>22</v>
       </c>
       <c r="I16" t="s">
-        <v>534</v>
-      </c>
-      <c r="J16" t="s">
-        <v>535</v>
+        <v>528</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>672</v>
       </c>
       <c r="K16" t="b">
         <v>1</v>
@@ -3090,10 +3087,10 @@
         <v>16</v>
       </c>
       <c r="I17" t="s">
-        <v>536</v>
-      </c>
-      <c r="J17" t="s">
-        <v>537</v>
+        <v>529</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>673</v>
       </c>
       <c r="K17" t="b">
         <v>1</v>
@@ -3130,10 +3127,10 @@
         <v>26</v>
       </c>
       <c r="I18" t="s">
-        <v>538</v>
-      </c>
-      <c r="J18" t="s">
-        <v>539</v>
+        <v>530</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>674</v>
       </c>
       <c r="K18" t="b">
         <v>1</v>
@@ -3170,10 +3167,10 @@
         <v>7</v>
       </c>
       <c r="I19" t="s">
-        <v>540</v>
-      </c>
-      <c r="J19" t="s">
-        <v>541</v>
+        <v>531</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>675</v>
       </c>
       <c r="K19" t="b">
         <v>1</v>
@@ -3210,10 +3207,10 @@
         <v>5</v>
       </c>
       <c r="I20" t="s">
-        <v>542</v>
-      </c>
-      <c r="J20" t="s">
-        <v>543</v>
+        <v>532</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>533</v>
       </c>
       <c r="K20" t="b">
         <v>1</v>
@@ -3250,10 +3247,10 @@
         <v>32</v>
       </c>
       <c r="I21" t="s">
-        <v>544</v>
-      </c>
-      <c r="J21" t="s">
-        <v>545</v>
+        <v>534</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>535</v>
       </c>
       <c r="K21" t="b">
         <v>1</v>
@@ -3290,10 +3287,10 @@
         <v>8</v>
       </c>
       <c r="I22" t="s">
-        <v>546</v>
-      </c>
-      <c r="J22" t="s">
-        <v>547</v>
+        <v>536</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>537</v>
       </c>
       <c r="K22" t="b">
         <v>1</v>
@@ -3330,10 +3327,10 @@
         <v>12</v>
       </c>
       <c r="I23" t="s">
-        <v>548</v>
-      </c>
-      <c r="J23" t="s">
-        <v>549</v>
+        <v>538</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>539</v>
       </c>
       <c r="K23" t="b">
         <v>1</v>
@@ -3370,10 +3367,10 @@
         <v>24</v>
       </c>
       <c r="I24" t="s">
-        <v>550</v>
-      </c>
-      <c r="J24" t="s">
-        <v>551</v>
+        <v>540</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>541</v>
       </c>
       <c r="K24" t="b">
         <v>1</v>
@@ -3410,10 +3407,10 @@
         <v>22</v>
       </c>
       <c r="I25" t="s">
-        <v>552</v>
-      </c>
-      <c r="J25" t="s">
-        <v>553</v>
+        <v>542</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>543</v>
       </c>
       <c r="K25" t="b">
         <v>1</v>
@@ -3450,10 +3447,10 @@
         <v>7</v>
       </c>
       <c r="I26" t="s">
-        <v>554</v>
-      </c>
-      <c r="J26" t="s">
-        <v>555</v>
+        <v>544</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>545</v>
       </c>
       <c r="K26" t="b">
         <v>1</v>
@@ -3490,10 +3487,10 @@
         <v>1</v>
       </c>
       <c r="I27" t="s">
-        <v>556</v>
-      </c>
-      <c r="J27" t="s">
-        <v>557</v>
+        <v>546</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>547</v>
       </c>
       <c r="K27" t="b">
         <v>1</v>
@@ -3530,10 +3527,10 @@
         <v>4</v>
       </c>
       <c r="I28" t="s">
-        <v>558</v>
-      </c>
-      <c r="J28" t="s">
-        <v>559</v>
+        <v>548</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>549</v>
       </c>
       <c r="K28" t="b">
         <v>1</v>
@@ -3570,10 +3567,10 @@
         <v>20</v>
       </c>
       <c r="I29" t="s">
-        <v>560</v>
-      </c>
-      <c r="J29" t="s">
-        <v>561</v>
+        <v>550</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>551</v>
       </c>
       <c r="K29" t="b">
         <v>1</v>
@@ -3610,10 +3607,10 @@
         <v>0</v>
       </c>
       <c r="I30" t="s">
-        <v>562</v>
-      </c>
-      <c r="J30" t="s">
-        <v>563</v>
+        <v>552</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>553</v>
       </c>
       <c r="K30" t="b">
         <v>1</v>
@@ -3650,10 +3647,10 @@
         <v>8</v>
       </c>
       <c r="I31" t="s">
-        <v>564</v>
-      </c>
-      <c r="J31" t="s">
-        <v>565</v>
+        <v>554</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>555</v>
       </c>
       <c r="K31" t="b">
         <v>1</v>
@@ -3690,10 +3687,10 @@
         <v>1</v>
       </c>
       <c r="I32" t="s">
-        <v>566</v>
-      </c>
-      <c r="J32" t="s">
-        <v>567</v>
+        <v>556</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>557</v>
       </c>
       <c r="K32" t="b">
         <v>1</v>
@@ -3730,10 +3727,10 @@
         <v>0</v>
       </c>
       <c r="I33" t="s">
-        <v>568</v>
-      </c>
-      <c r="J33" t="s">
-        <v>569</v>
+        <v>558</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>559</v>
       </c>
       <c r="K33" t="b">
         <v>1</v>
@@ -3770,10 +3767,10 @@
         <v>3</v>
       </c>
       <c r="I34" t="s">
-        <v>570</v>
-      </c>
-      <c r="J34" t="s">
-        <v>571</v>
+        <v>560</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>561</v>
       </c>
       <c r="K34" t="b">
         <v>1</v>
@@ -3784,13 +3781,16 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>671</v>
+        <v>659</v>
       </c>
       <c r="D35" t="s">
         <v>97</v>
       </c>
-      <c r="J35" t="s">
-        <v>679</v>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>676</v>
       </c>
       <c r="K35" t="b">
         <v>0</v>
@@ -3827,10 +3827,10 @@
         <v>21</v>
       </c>
       <c r="I36" t="s">
-        <v>572</v>
-      </c>
-      <c r="J36" t="s">
-        <v>573</v>
+        <v>562</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>563</v>
       </c>
       <c r="K36" t="b">
         <v>1</v>
@@ -3867,10 +3867,10 @@
         <v>4</v>
       </c>
       <c r="I37" t="s">
-        <v>574</v>
-      </c>
-      <c r="J37" t="s">
-        <v>575</v>
+        <v>564</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>565</v>
       </c>
       <c r="K37" t="b">
         <v>1</v>
@@ -3907,10 +3907,10 @@
         <v>0</v>
       </c>
       <c r="I38" t="s">
-        <v>576</v>
-      </c>
-      <c r="J38" t="s">
-        <v>577</v>
+        <v>566</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>567</v>
       </c>
       <c r="K38" t="b">
         <v>1</v>
@@ -3947,10 +3947,10 @@
         <v>1</v>
       </c>
       <c r="I39" t="s">
-        <v>578</v>
-      </c>
-      <c r="J39" t="s">
-        <v>579</v>
+        <v>568</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>569</v>
       </c>
       <c r="K39" t="b">
         <v>1</v>
@@ -3987,10 +3987,10 @@
         <v>4</v>
       </c>
       <c r="I40" t="s">
-        <v>580</v>
-      </c>
-      <c r="J40" t="s">
-        <v>581</v>
+        <v>570</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>571</v>
       </c>
       <c r="K40" t="b">
         <v>1</v>
@@ -4027,10 +4027,10 @@
         <v>7</v>
       </c>
       <c r="I41" t="s">
-        <v>582</v>
-      </c>
-      <c r="J41" t="s">
-        <v>583</v>
+        <v>572</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>573</v>
       </c>
       <c r="K41" t="b">
         <v>1</v>
@@ -4067,10 +4067,10 @@
         <v>14</v>
       </c>
       <c r="I42" t="s">
-        <v>584</v>
-      </c>
-      <c r="J42" t="s">
-        <v>585</v>
+        <v>574</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>575</v>
       </c>
       <c r="K42" t="b">
         <v>1</v>
@@ -4107,10 +4107,10 @@
         <v>2</v>
       </c>
       <c r="I43" t="s">
-        <v>586</v>
-      </c>
-      <c r="J43" t="s">
-        <v>587</v>
+        <v>576</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>577</v>
       </c>
       <c r="K43" t="b">
         <v>1</v>
@@ -4147,10 +4147,10 @@
         <v>0</v>
       </c>
       <c r="I44" t="s">
-        <v>588</v>
-      </c>
-      <c r="J44" t="s">
-        <v>589</v>
+        <v>578</v>
+      </c>
+      <c r="J44" s="1" t="s">
+        <v>579</v>
       </c>
       <c r="K44" t="b">
         <v>1</v>
@@ -4187,10 +4187,10 @@
         <v>13</v>
       </c>
       <c r="I45" t="s">
-        <v>590</v>
-      </c>
-      <c r="J45" t="s">
-        <v>591</v>
+        <v>580</v>
+      </c>
+      <c r="J45" s="1" t="s">
+        <v>581</v>
       </c>
       <c r="K45" t="b">
         <v>1</v>
@@ -4227,10 +4227,10 @@
         <v>0</v>
       </c>
       <c r="I46" t="s">
-        <v>593</v>
-      </c>
-      <c r="J46" t="s">
-        <v>592</v>
+        <v>583</v>
+      </c>
+      <c r="J46" s="1" t="s">
+        <v>582</v>
       </c>
       <c r="K46" t="b">
         <v>1</v>
@@ -4241,7 +4241,7 @@
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>672</v>
+        <v>660</v>
       </c>
       <c r="D47" t="s">
         <v>135</v>
@@ -4260,8 +4260,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J47" t="s">
-        <v>673</v>
+      <c r="J47" s="1" t="s">
+        <v>677</v>
       </c>
       <c r="K47" t="b">
         <v>0</v>
@@ -4298,10 +4298,10 @@
         <v>22</v>
       </c>
       <c r="I48" t="s">
-        <v>594</v>
-      </c>
-      <c r="J48" t="s">
-        <v>595</v>
+        <v>584</v>
+      </c>
+      <c r="J48" s="1" t="s">
+        <v>585</v>
       </c>
       <c r="K48" t="b">
         <v>1</v>
@@ -4338,10 +4338,10 @@
         <v>0</v>
       </c>
       <c r="I49" t="s">
-        <v>596</v>
-      </c>
-      <c r="J49" t="s">
-        <v>597</v>
+        <v>586</v>
+      </c>
+      <c r="J49" s="1" t="s">
+        <v>587</v>
       </c>
       <c r="K49" t="b">
         <v>1</v>
@@ -4378,10 +4378,10 @@
         <v>11</v>
       </c>
       <c r="I50" t="s">
-        <v>598</v>
-      </c>
-      <c r="J50" t="s">
-        <v>599</v>
+        <v>588</v>
+      </c>
+      <c r="J50" s="1" t="s">
+        <v>589</v>
       </c>
       <c r="K50" t="b">
         <v>1</v>
@@ -4418,10 +4418,10 @@
         <v>6</v>
       </c>
       <c r="I51" t="s">
-        <v>600</v>
-      </c>
-      <c r="J51" t="s">
-        <v>601</v>
+        <v>590</v>
+      </c>
+      <c r="J51" s="1" t="s">
+        <v>591</v>
       </c>
       <c r="K51" t="b">
         <v>1</v>
@@ -4458,10 +4458,10 @@
         <v>0</v>
       </c>
       <c r="I52" t="s">
-        <v>602</v>
-      </c>
-      <c r="J52" t="s">
-        <v>603</v>
+        <v>592</v>
+      </c>
+      <c r="J52" s="1" t="s">
+        <v>593</v>
       </c>
       <c r="K52" t="b">
         <v>1</v>
@@ -4498,10 +4498,10 @@
         <v>0</v>
       </c>
       <c r="I53" t="s">
-        <v>604</v>
-      </c>
-      <c r="J53" t="s">
-        <v>605</v>
+        <v>594</v>
+      </c>
+      <c r="J53" s="1" t="s">
+        <v>595</v>
       </c>
       <c r="K53" t="b">
         <v>1</v>
@@ -4538,10 +4538,10 @@
         <v>1</v>
       </c>
       <c r="I54" t="s">
-        <v>606</v>
-      </c>
-      <c r="J54" t="s">
-        <v>607</v>
+        <v>596</v>
+      </c>
+      <c r="J54" s="1" t="s">
+        <v>597</v>
       </c>
       <c r="K54" t="b">
         <v>1</v>
@@ -4578,10 +4578,10 @@
         <v>10</v>
       </c>
       <c r="I55" t="s">
-        <v>680</v>
-      </c>
-      <c r="J55" t="s">
-        <v>608</v>
+        <v>665</v>
+      </c>
+      <c r="J55" s="1" t="s">
+        <v>598</v>
       </c>
       <c r="K55" t="b">
         <v>1</v>
@@ -4618,10 +4618,10 @@
         <v>29</v>
       </c>
       <c r="I56" t="s">
-        <v>609</v>
-      </c>
-      <c r="J56" t="s">
-        <v>610</v>
+        <v>599</v>
+      </c>
+      <c r="J56" s="1" t="s">
+        <v>600</v>
       </c>
       <c r="K56" t="b">
         <v>1</v>
@@ -4658,10 +4658,10 @@
         <v>15</v>
       </c>
       <c r="I57" t="s">
-        <v>611</v>
-      </c>
-      <c r="J57" t="s">
-        <v>612</v>
+        <v>601</v>
+      </c>
+      <c r="J57" s="1" t="s">
+        <v>602</v>
       </c>
       <c r="K57" t="b">
         <v>1</v>
@@ -4698,10 +4698,10 @@
         <v>9</v>
       </c>
       <c r="I58" t="s">
-        <v>613</v>
-      </c>
-      <c r="J58" t="s">
-        <v>614</v>
+        <v>603</v>
+      </c>
+      <c r="J58" s="1" t="s">
+        <v>604</v>
       </c>
       <c r="K58" t="b">
         <v>1</v>
@@ -4738,10 +4738,10 @@
         <v>7</v>
       </c>
       <c r="I59" t="s">
-        <v>615</v>
-      </c>
-      <c r="J59" t="s">
-        <v>616</v>
+        <v>605</v>
+      </c>
+      <c r="J59" s="1" t="s">
+        <v>606</v>
       </c>
       <c r="K59" t="b">
         <v>1</v>
@@ -4752,7 +4752,7 @@
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>617</v>
+        <v>607</v>
       </c>
       <c r="D60" t="s">
         <v>180</v>
@@ -4772,10 +4772,10 @@
         <v>0</v>
       </c>
       <c r="I60" t="s">
-        <v>618</v>
-      </c>
-      <c r="J60" t="s">
-        <v>619</v>
+        <v>608</v>
+      </c>
+      <c r="J60" s="1" t="s">
+        <v>609</v>
       </c>
       <c r="K60" t="b">
         <v>0</v>
@@ -4786,7 +4786,7 @@
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>620</v>
+        <v>610</v>
       </c>
       <c r="D61" t="s">
         <v>180</v>
@@ -4803,10 +4803,10 @@
         <v>0</v>
       </c>
       <c r="I61" t="s">
-        <v>621</v>
-      </c>
-      <c r="J61" t="s">
-        <v>622</v>
+        <v>611</v>
+      </c>
+      <c r="J61" s="1" t="s">
+        <v>678</v>
       </c>
       <c r="K61" t="b">
         <v>0</v>
@@ -4843,10 +4843,10 @@
         <v>21</v>
       </c>
       <c r="I62" t="s">
-        <v>623</v>
-      </c>
-      <c r="J62" t="s">
-        <v>624</v>
+        <v>612</v>
+      </c>
+      <c r="J62" s="1" t="s">
+        <v>613</v>
       </c>
       <c r="K62" t="b">
         <v>1</v>
@@ -4857,7 +4857,7 @@
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>633</v>
+        <v>622</v>
       </c>
       <c r="D63" t="s">
         <v>190</v>
@@ -4874,10 +4874,10 @@
         <v>0</v>
       </c>
       <c r="I63" t="s">
-        <v>635</v>
-      </c>
-      <c r="J63" t="s">
-        <v>636</v>
+        <v>624</v>
+      </c>
+      <c r="J63" s="1" t="s">
+        <v>625</v>
       </c>
       <c r="K63" t="b">
         <v>0</v>
@@ -4914,10 +4914,10 @@
         <v>3</v>
       </c>
       <c r="I64" t="s">
-        <v>625</v>
-      </c>
-      <c r="J64" t="s">
-        <v>626</v>
+        <v>614</v>
+      </c>
+      <c r="J64" s="1" t="s">
+        <v>615</v>
       </c>
       <c r="K64" t="b">
         <v>1</v>
@@ -4954,10 +4954,10 @@
         <v>10</v>
       </c>
       <c r="I65" t="s">
-        <v>627</v>
-      </c>
-      <c r="J65" t="s">
-        <v>628</v>
+        <v>616</v>
+      </c>
+      <c r="J65" s="1" t="s">
+        <v>617</v>
       </c>
       <c r="K65" t="b">
         <v>1</v>
@@ -4994,10 +4994,10 @@
         <v>0</v>
       </c>
       <c r="I66" t="s">
-        <v>629</v>
-      </c>
-      <c r="J66" t="s">
-        <v>630</v>
+        <v>618</v>
+      </c>
+      <c r="J66" s="1" t="s">
+        <v>619</v>
       </c>
       <c r="K66" t="b">
         <v>1</v>
@@ -5008,7 +5008,7 @@
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>634</v>
+        <v>623</v>
       </c>
       <c r="D67" t="s">
         <v>190</v>
@@ -5025,10 +5025,10 @@
         <v>0</v>
       </c>
       <c r="I67" t="s">
-        <v>631</v>
-      </c>
-      <c r="J67" t="s">
-        <v>632</v>
+        <v>620</v>
+      </c>
+      <c r="J67" s="1" t="s">
+        <v>621</v>
       </c>
       <c r="K67" t="b">
         <v>0</v>
@@ -5065,10 +5065,10 @@
         <v>15</v>
       </c>
       <c r="I68" t="s">
-        <v>637</v>
-      </c>
-      <c r="J68" t="s">
-        <v>638</v>
+        <v>626</v>
+      </c>
+      <c r="J68" s="1" t="s">
+        <v>627</v>
       </c>
       <c r="K68" t="b">
         <v>1</v>
@@ -5105,10 +5105,10 @@
         <v>11</v>
       </c>
       <c r="I69" t="s">
-        <v>639</v>
-      </c>
-      <c r="J69" t="s">
-        <v>640</v>
+        <v>628</v>
+      </c>
+      <c r="J69" s="1" t="s">
+        <v>629</v>
       </c>
       <c r="K69" t="b">
         <v>1</v>
@@ -5145,10 +5145,10 @@
         <v>4</v>
       </c>
       <c r="I70" t="s">
-        <v>641</v>
-      </c>
-      <c r="J70" t="s">
-        <v>642</v>
+        <v>630</v>
+      </c>
+      <c r="J70" s="1" t="s">
+        <v>631</v>
       </c>
       <c r="K70" t="b">
         <v>1</v>
@@ -5185,10 +5185,10 @@
         <v>10</v>
       </c>
       <c r="I71" t="s">
-        <v>643</v>
-      </c>
-      <c r="J71" t="s">
-        <v>644</v>
+        <v>632</v>
+      </c>
+      <c r="J71" s="1" t="s">
+        <v>633</v>
       </c>
       <c r="K71" t="b">
         <v>1</v>
@@ -5225,10 +5225,10 @@
         <v>0</v>
       </c>
       <c r="I72" t="s">
-        <v>645</v>
-      </c>
-      <c r="J72" t="s">
-        <v>646</v>
+        <v>634</v>
+      </c>
+      <c r="J72" s="1" t="s">
+        <v>635</v>
       </c>
       <c r="K72" t="b">
         <v>1</v>
@@ -5239,7 +5239,7 @@
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>647</v>
+        <v>636</v>
       </c>
       <c r="D73" t="s">
         <v>203</v>
@@ -5256,10 +5256,10 @@
         <v>0</v>
       </c>
       <c r="I73" t="s">
-        <v>648</v>
-      </c>
-      <c r="J73" t="s">
-        <v>649</v>
+        <v>637</v>
+      </c>
+      <c r="J73" s="1" t="s">
+        <v>679</v>
       </c>
       <c r="K73" t="b">
         <v>0</v>
@@ -5296,10 +5296,10 @@
         <v>26</v>
       </c>
       <c r="I74" t="s">
-        <v>650</v>
-      </c>
-      <c r="J74" t="s">
-        <v>651</v>
+        <v>638</v>
+      </c>
+      <c r="J74" s="1" t="s">
+        <v>639</v>
       </c>
       <c r="K74" t="b">
         <v>1</v>
@@ -5310,7 +5310,7 @@
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>656</v>
+        <v>644</v>
       </c>
       <c r="D75" t="s">
         <v>219</v>
@@ -5327,10 +5327,10 @@
         <v>0</v>
       </c>
       <c r="I75" t="s">
-        <v>657</v>
-      </c>
-      <c r="J75" t="s">
-        <v>658</v>
+        <v>645</v>
+      </c>
+      <c r="J75" s="1" t="s">
+        <v>646</v>
       </c>
       <c r="K75" t="b">
         <v>0</v>
@@ -5367,10 +5367,10 @@
         <v>5</v>
       </c>
       <c r="I76" t="s">
-        <v>652</v>
-      </c>
-      <c r="J76" t="s">
-        <v>653</v>
+        <v>640</v>
+      </c>
+      <c r="J76" s="1" t="s">
+        <v>641</v>
       </c>
       <c r="K76" t="b">
         <v>1</v>
@@ -5407,10 +5407,10 @@
         <v>8</v>
       </c>
       <c r="I77" t="s">
-        <v>654</v>
-      </c>
-      <c r="J77" t="s">
-        <v>655</v>
+        <v>642</v>
+      </c>
+      <c r="J77" s="1" t="s">
+        <v>643</v>
       </c>
       <c r="K77" t="b">
         <v>1</v>
@@ -5447,10 +5447,10 @@
         <v>0</v>
       </c>
       <c r="I78" t="s">
-        <v>659</v>
-      </c>
-      <c r="J78" t="s">
-        <v>660</v>
+        <v>647</v>
+      </c>
+      <c r="J78" s="1" t="s">
+        <v>648</v>
       </c>
       <c r="K78" t="b">
         <v>1</v>
@@ -5487,10 +5487,10 @@
         <v>6</v>
       </c>
       <c r="I79" t="s">
-        <v>661</v>
-      </c>
-      <c r="J79" t="s">
-        <v>662</v>
+        <v>649</v>
+      </c>
+      <c r="J79" s="1" t="s">
+        <v>650</v>
       </c>
       <c r="K79" t="b">
         <v>1</v>
@@ -5527,10 +5527,10 @@
         <v>24</v>
       </c>
       <c r="I80" t="s">
-        <v>663</v>
-      </c>
-      <c r="J80" t="s">
-        <v>664</v>
+        <v>651</v>
+      </c>
+      <c r="J80" s="1" t="s">
+        <v>652</v>
       </c>
       <c r="K80" t="b">
         <v>1</v>
@@ -5567,10 +5567,10 @@
         <v>0</v>
       </c>
       <c r="I81" t="s">
-        <v>665</v>
-      </c>
-      <c r="J81" t="s">
-        <v>666</v>
+        <v>653</v>
+      </c>
+      <c r="J81" s="1" t="s">
+        <v>654</v>
       </c>
       <c r="K81" t="b">
         <v>1</v>
@@ -5607,10 +5607,10 @@
         <v>4</v>
       </c>
       <c r="I82" t="s">
-        <v>668</v>
-      </c>
-      <c r="J82" t="s">
-        <v>667</v>
+        <v>656</v>
+      </c>
+      <c r="J82" s="1" t="s">
+        <v>655</v>
       </c>
       <c r="K82" t="b">
         <v>1</v>
@@ -5647,10 +5647,10 @@
         <v>0</v>
       </c>
       <c r="I83" t="s">
-        <v>669</v>
-      </c>
-      <c r="J83" t="s">
-        <v>670</v>
+        <v>657</v>
+      </c>
+      <c r="J83" s="1" t="s">
+        <v>658</v>
       </c>
       <c r="K83" t="b">
         <v>1</v>
@@ -5935,10 +5935,10 @@
         <v>11</v>
       </c>
       <c r="I92" t="s">
-        <v>456</v>
-      </c>
-      <c r="J92" t="s">
         <v>455</v>
+      </c>
+      <c r="J92" s="1" t="s">
+        <v>454</v>
       </c>
       <c r="K92" t="b">
         <v>1</v>
@@ -5975,10 +5975,10 @@
         <v>4</v>
       </c>
       <c r="I93" t="s">
-        <v>458</v>
-      </c>
-      <c r="J93" t="s">
         <v>457</v>
+      </c>
+      <c r="J93" s="1" t="s">
+        <v>456</v>
       </c>
       <c r="K93" t="b">
         <v>1</v>
@@ -6015,10 +6015,10 @@
         <v>0</v>
       </c>
       <c r="I94" t="s">
-        <v>460</v>
-      </c>
-      <c r="J94" t="s">
         <v>459</v>
+      </c>
+      <c r="J94" s="1" t="s">
+        <v>458</v>
       </c>
       <c r="K94" t="b">
         <v>1</v>
@@ -6055,10 +6055,10 @@
         <v>10</v>
       </c>
       <c r="I95" t="s">
-        <v>462</v>
-      </c>
-      <c r="J95" t="s">
         <v>461</v>
+      </c>
+      <c r="J95" s="1" t="s">
+        <v>460</v>
       </c>
       <c r="K95" t="b">
         <v>1</v>
@@ -6095,10 +6095,10 @@
         <v>14</v>
       </c>
       <c r="I96" t="s">
-        <v>464</v>
-      </c>
-      <c r="J96" t="s">
         <v>463</v>
+      </c>
+      <c r="J96" s="1" t="s">
+        <v>462</v>
       </c>
       <c r="K96" t="b">
         <v>1</v>
@@ -6135,10 +6135,10 @@
         <v>2</v>
       </c>
       <c r="I97" t="s">
-        <v>446</v>
-      </c>
-      <c r="J97" t="s">
         <v>445</v>
+      </c>
+      <c r="J97" s="1" t="s">
+        <v>444</v>
       </c>
       <c r="K97" t="b">
         <v>1</v>
@@ -6175,10 +6175,10 @@
         <v>0</v>
       </c>
       <c r="I98" t="s">
-        <v>448</v>
-      </c>
-      <c r="J98" t="s">
         <v>447</v>
+      </c>
+      <c r="J98" s="1" t="s">
+        <v>446</v>
       </c>
       <c r="K98" t="b">
         <v>1</v>
@@ -6215,10 +6215,10 @@
         <v>6</v>
       </c>
       <c r="I99" t="s">
-        <v>450</v>
-      </c>
-      <c r="J99" t="s">
         <v>449</v>
+      </c>
+      <c r="J99" s="1" t="s">
+        <v>448</v>
       </c>
       <c r="K99" t="b">
         <v>1</v>
@@ -6255,10 +6255,10 @@
         <v>3</v>
       </c>
       <c r="I100" t="s">
-        <v>452</v>
-      </c>
-      <c r="J100" t="s">
         <v>451</v>
+      </c>
+      <c r="J100" s="1" t="s">
+        <v>450</v>
       </c>
       <c r="K100" t="b">
         <v>1</v>
@@ -6295,10 +6295,10 @@
         <v>20</v>
       </c>
       <c r="I101" t="s">
-        <v>454</v>
-      </c>
-      <c r="J101" t="s">
         <v>453</v>
+      </c>
+      <c r="J101" s="1" t="s">
+        <v>452</v>
       </c>
       <c r="K101" t="b">
         <v>1</v>
@@ -6335,10 +6335,10 @@
         <v>30</v>
       </c>
       <c r="I102" t="s">
-        <v>436</v>
-      </c>
-      <c r="J102" t="s">
         <v>435</v>
+      </c>
+      <c r="J102" s="1" t="s">
+        <v>669</v>
       </c>
       <c r="K102" t="b">
         <v>1</v>
@@ -6377,7 +6377,7 @@
       <c r="I103" t="s">
         <v>432</v>
       </c>
-      <c r="J103" t="s">
+      <c r="J103" s="1" t="s">
         <v>431</v>
       </c>
       <c r="K103" t="b">
@@ -6415,10 +6415,10 @@
         <v>0</v>
       </c>
       <c r="I104" t="s">
-        <v>438</v>
-      </c>
-      <c r="J104" t="s">
         <v>437</v>
+      </c>
+      <c r="J104" s="1" t="s">
+        <v>436</v>
       </c>
       <c r="K104" t="b">
         <v>1</v>
@@ -6457,7 +6457,7 @@
       <c r="I105" t="s">
         <v>428</v>
       </c>
-      <c r="J105" t="s">
+      <c r="J105" s="1" t="s">
         <v>427</v>
       </c>
       <c r="K105" t="b">
@@ -6497,7 +6497,7 @@
       <c r="I106" t="s">
         <v>430</v>
       </c>
-      <c r="J106" t="s">
+      <c r="J106" s="1" t="s">
         <v>429</v>
       </c>
       <c r="K106" t="b">
@@ -6537,7 +6537,7 @@
       <c r="I107" t="s">
         <v>434</v>
       </c>
-      <c r="J107" t="s">
+      <c r="J107" s="1" t="s">
         <v>433</v>
       </c>
       <c r="K107" t="b">
@@ -6575,10 +6575,10 @@
         <v>22</v>
       </c>
       <c r="I108" t="s">
-        <v>490</v>
-      </c>
-      <c r="J108" t="s">
-        <v>489</v>
+        <v>488</v>
+      </c>
+      <c r="J108" s="1" t="s">
+        <v>487</v>
       </c>
       <c r="K108" t="b">
         <v>1</v>
@@ -6615,10 +6615,10 @@
         <v>8</v>
       </c>
       <c r="I109" t="s">
-        <v>492</v>
-      </c>
-      <c r="J109" t="s">
-        <v>491</v>
+        <v>490</v>
+      </c>
+      <c r="J109" s="1" t="s">
+        <v>489</v>
       </c>
       <c r="K109" t="b">
         <v>1</v>
@@ -6655,10 +6655,10 @@
         <v>9</v>
       </c>
       <c r="I110" t="s">
-        <v>494</v>
-      </c>
-      <c r="J110" t="s">
-        <v>493</v>
+        <v>492</v>
+      </c>
+      <c r="J110" s="1" t="s">
+        <v>491</v>
       </c>
       <c r="K110" t="b">
         <v>1</v>
@@ -6695,10 +6695,10 @@
         <v>18</v>
       </c>
       <c r="I111" t="s">
-        <v>472</v>
-      </c>
-      <c r="J111" t="s">
         <v>471</v>
+      </c>
+      <c r="J111" s="1" t="s">
+        <v>470</v>
       </c>
       <c r="K111" t="b">
         <v>1</v>
@@ -6735,10 +6735,10 @@
         <v>3</v>
       </c>
       <c r="I112" t="s">
-        <v>474</v>
-      </c>
-      <c r="J112" t="s">
         <v>473</v>
+      </c>
+      <c r="J112" s="1" t="s">
+        <v>472</v>
       </c>
       <c r="K112" t="b">
         <v>1</v>
@@ -6775,10 +6775,10 @@
         <v>14</v>
       </c>
       <c r="I113" t="s">
-        <v>476</v>
-      </c>
-      <c r="J113" t="s">
         <v>475</v>
+      </c>
+      <c r="J113" s="1" t="s">
+        <v>474</v>
       </c>
       <c r="K113" t="b">
         <v>1</v>
@@ -6815,10 +6815,10 @@
         <v>3</v>
       </c>
       <c r="I114" t="s">
-        <v>478</v>
-      </c>
-      <c r="J114" t="s">
         <v>477</v>
+      </c>
+      <c r="J114" s="1" t="s">
+        <v>476</v>
       </c>
       <c r="K114" t="b">
         <v>1</v>
@@ -6855,10 +6855,10 @@
         <v>16</v>
       </c>
       <c r="I115" t="s">
-        <v>440</v>
-      </c>
-      <c r="J115" t="s">
         <v>439</v>
+      </c>
+      <c r="J115" s="1" t="s">
+        <v>438</v>
       </c>
       <c r="K115" t="b">
         <v>1</v>
@@ -6895,10 +6895,10 @@
         <v>14</v>
       </c>
       <c r="I116" t="s">
-        <v>442</v>
-      </c>
-      <c r="J116" t="s">
         <v>441</v>
+      </c>
+      <c r="J116" s="1" t="s">
+        <v>440</v>
       </c>
       <c r="K116" t="b">
         <v>1</v>
@@ -6935,10 +6935,10 @@
         <v>7</v>
       </c>
       <c r="I117" t="s">
-        <v>444</v>
-      </c>
-      <c r="J117" t="s">
         <v>443</v>
+      </c>
+      <c r="J117" s="1" t="s">
+        <v>442</v>
       </c>
       <c r="K117" t="b">
         <v>1</v>
@@ -6975,10 +6975,10 @@
         <v>12</v>
       </c>
       <c r="I118" t="s">
-        <v>466</v>
-      </c>
-      <c r="J118" t="s">
         <v>465</v>
+      </c>
+      <c r="J118" s="1" t="s">
+        <v>464</v>
       </c>
       <c r="K118" t="b">
         <v>1</v>
@@ -7015,10 +7015,10 @@
         <v>12</v>
       </c>
       <c r="I119" t="s">
-        <v>468</v>
-      </c>
-      <c r="J119" t="s">
         <v>467</v>
+      </c>
+      <c r="J119" s="1" t="s">
+        <v>466</v>
       </c>
       <c r="K119" t="b">
         <v>1</v>
@@ -7055,10 +7055,10 @@
         <v>13</v>
       </c>
       <c r="I120" t="s">
-        <v>470</v>
-      </c>
-      <c r="J120" t="s">
         <v>469</v>
+      </c>
+      <c r="J120" s="1" t="s">
+        <v>468</v>
       </c>
       <c r="K120" t="b">
         <v>1</v>
@@ -7097,7 +7097,7 @@
       <c r="I121" t="s">
         <v>424</v>
       </c>
-      <c r="J121" t="s">
+      <c r="J121" s="1" t="s">
         <v>423</v>
       </c>
       <c r="K121" t="b">
@@ -7137,7 +7137,7 @@
       <c r="I122" t="s">
         <v>426</v>
       </c>
-      <c r="J122" t="s">
+      <c r="J122" s="1" t="s">
         <v>425</v>
       </c>
       <c r="K122" t="b">
@@ -7177,7 +7177,7 @@
       <c r="I123" t="s">
         <v>420</v>
       </c>
-      <c r="J123" t="s">
+      <c r="J123" s="1" t="s">
         <v>419</v>
       </c>
       <c r="K123" t="b">
@@ -7217,7 +7217,7 @@
       <c r="I124" t="s">
         <v>422</v>
       </c>
-      <c r="J124" t="s">
+      <c r="J124" s="1" t="s">
         <v>421</v>
       </c>
       <c r="K124" t="b">
@@ -7257,7 +7257,7 @@
       <c r="I125" t="s">
         <v>416</v>
       </c>
-      <c r="J125" t="s">
+      <c r="J125" s="1" t="s">
         <v>415</v>
       </c>
       <c r="K125" t="b">
@@ -7297,7 +7297,7 @@
       <c r="I126" t="s">
         <v>418</v>
       </c>
-      <c r="J126" t="s">
+      <c r="J126" s="1" t="s">
         <v>417</v>
       </c>
       <c r="K126" t="b">
@@ -7337,7 +7337,7 @@
       <c r="I127" t="s">
         <v>412</v>
       </c>
-      <c r="J127" t="s">
+      <c r="J127" s="1" t="s">
         <v>411</v>
       </c>
       <c r="K127" t="b">
@@ -7377,7 +7377,7 @@
       <c r="I128" t="s">
         <v>414</v>
       </c>
-      <c r="J128" t="s">
+      <c r="J128" s="1" t="s">
         <v>413</v>
       </c>
       <c r="K128" t="b">
@@ -7415,10 +7415,10 @@
         <v>11</v>
       </c>
       <c r="I129" t="s">
-        <v>480</v>
-      </c>
-      <c r="J129" t="s">
         <v>479</v>
+      </c>
+      <c r="J129" s="1" t="s">
+        <v>478</v>
       </c>
       <c r="K129" t="b">
         <v>1</v>
@@ -7455,10 +7455,10 @@
         <v>7</v>
       </c>
       <c r="I130" t="s">
-        <v>482</v>
-      </c>
-      <c r="J130" t="s">
         <v>481</v>
+      </c>
+      <c r="J130" s="1" t="s">
+        <v>480</v>
       </c>
       <c r="K130" t="b">
         <v>1</v>
@@ -7495,10 +7495,10 @@
         <v>7</v>
       </c>
       <c r="I131" t="s">
-        <v>484</v>
-      </c>
-      <c r="J131" t="s">
         <v>483</v>
+      </c>
+      <c r="J131" s="1" t="s">
+        <v>482</v>
       </c>
       <c r="K131" t="b">
         <v>1</v>
@@ -7535,10 +7535,10 @@
         <v>5</v>
       </c>
       <c r="I132" t="s">
-        <v>486</v>
-      </c>
-      <c r="J132" t="s">
-        <v>485</v>
+        <v>484</v>
+      </c>
+      <c r="J132" s="1" t="s">
+        <v>666</v>
       </c>
       <c r="K132" t="b">
         <v>1</v>
@@ -7575,10 +7575,10 @@
         <v>1</v>
       </c>
       <c r="I133" t="s">
-        <v>488</v>
-      </c>
-      <c r="J133" t="s">
-        <v>487</v>
+        <v>486</v>
+      </c>
+      <c r="J133" s="1" t="s">
+        <v>485</v>
       </c>
       <c r="K133" t="b">
         <v>1</v>
@@ -7589,13 +7589,16 @@
     </row>
     <row r="134" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="D134" t="s">
         <v>396</v>
       </c>
-      <c r="J134" t="s">
-        <v>507</v>
+      <c r="E134">
+        <v>0</v>
+      </c>
+      <c r="J134" s="1" t="s">
+        <v>667</v>
       </c>
       <c r="K134" t="b">
         <v>0</v>
@@ -7606,13 +7609,16 @@
     </row>
     <row r="135" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="D135" t="s">
         <v>358</v>
       </c>
-      <c r="J135" t="s">
-        <v>500</v>
+      <c r="E135">
+        <v>0</v>
+      </c>
+      <c r="J135" s="1" t="s">
+        <v>497</v>
       </c>
       <c r="K135" t="b">
         <v>0</v>
@@ -7623,13 +7629,16 @@
     </row>
     <row r="136" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="D136" t="s">
         <v>358</v>
       </c>
-      <c r="J136" t="s">
-        <v>499</v>
+      <c r="E136">
+        <v>0</v>
+      </c>
+      <c r="J136" s="1" t="s">
+        <v>668</v>
       </c>
       <c r="K136" t="b">
         <v>0</v>
@@ -7640,13 +7649,16 @@
     </row>
     <row r="137" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>309</v>
+        <v>498</v>
       </c>
       <c r="D137" t="s">
-        <v>305</v>
-      </c>
-      <c r="J137" t="s">
-        <v>501</v>
+        <v>315</v>
+      </c>
+      <c r="E137">
+        <v>0</v>
+      </c>
+      <c r="J137" s="1" t="s">
+        <v>499</v>
       </c>
       <c r="K137" t="b">
         <v>0</v>
@@ -7660,32 +7672,18 @@
         <v>502</v>
       </c>
       <c r="D138" t="s">
-        <v>315</v>
-      </c>
-      <c r="J138" t="s">
-        <v>503</v>
+        <v>273</v>
+      </c>
+      <c r="E138">
+        <v>0</v>
+      </c>
+      <c r="J138" s="1" t="s">
+        <v>501</v>
       </c>
       <c r="K138" t="b">
         <v>0</v>
       </c>
       <c r="L138" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A139" t="s">
-        <v>506</v>
-      </c>
-      <c r="D139" t="s">
-        <v>273</v>
-      </c>
-      <c r="J139" t="s">
-        <v>505</v>
-      </c>
-      <c r="K139" t="b">
-        <v>0</v>
-      </c>
-      <c r="L139" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>